<commit_message>
Level 4 properly added to list table
</commit_message>
<xml_diff>
--- a/Content/Assets/AlienDatatables/Spreadsheets/AlienList.xlsx
+++ b/Content/Assets/AlienDatatables/Spreadsheets/AlienList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halvo\Documents\Github\Blargon Jargon\Brain-Fog-Bachelor\Content\Assets\AlienDatatables\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AA856C-8F2A-47D6-ADFE-1713A5FC7E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAD1BEB-58F9-413D-9BD6-D01A66447019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A69FB867-82C4-40EA-BBD7-09F10CDC28A6}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{A69FB867-82C4-40EA-BBD7-09F10CDC28A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Alien</t>
   </si>
@@ -70,6 +70,13 @@
   </si>
   <si>
     <t>"AnimBlueprint'/Game/Assets/3D/Yoppoppo_Generic/AnimationBP_Generic.AnimationBP_Generic'"</t>
+  </si>
+  <si>
+    <t>"DataTable'/Game/Assets/AlienDatatables/Level1-4_AlienData.Level1-4_AlienData'"</t>
+  </si>
+  <si>
+    <t>A Yoppoppo traveler arrives, looking somewhat pained. It seems to be in a rush!
+"Skroog... Weddi Skroog?"</t>
   </si>
 </sst>
 </file>
@@ -424,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9552B152-2783-43C2-A1AD-B23D2F48934B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +513,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes from Feedback Implemented
</commit_message>
<xml_diff>
--- a/Content/Assets/AlienDatatables/Spreadsheets/AlienList.xlsx
+++ b/Content/Assets/AlienDatatables/Spreadsheets/AlienList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\Blargon Jargon\Brain-Fog-Bachelor\Content\Assets\AlienDatatables\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexa\Documents\GitHub\Brain-Fog-Bachelor\Content\Assets\AlienDatatables\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF6E17B-167F-48D6-8EA5-2B4CD65B2BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2CE87A-FF1F-43A0-B9A9-FDB308E2133E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A69FB867-82C4-40EA-BBD7-09F10CDC28A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A69FB867-82C4-40EA-BBD7-09F10CDC28A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Alien</t>
   </si>
@@ -82,7 +82,19 @@
     <t>"DataTable'/Game/Assets/AlienDatatables/Level1-5_AlienData.Level1-5_AlienData'"</t>
   </si>
   <si>
-    <t>(Insert angry yoppoppo line here)</t>
+    <t>A Yoppoppo traveler arrives. It squints at you.
+"Waiwai, Doob Belbo."</t>
+  </si>
+  <si>
+    <t>A Yoppoppo traveler arrives. It blushes and waves at you.
+"Waiwai, Belbo..."</t>
+  </si>
+  <si>
+    <t>A Yoppoppo traveler arrives and waves at you.
+"Waiwai, Belbo!"</t>
+  </si>
+  <si>
+    <t>StartingAnimation</t>
   </si>
 </sst>
 </file>
@@ -437,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9552B152-2783-43C2-A1AD-B23D2F48934B}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,9 +461,10 @@
     <col min="3" max="3" width="90.5703125" customWidth="1"/>
     <col min="4" max="4" width="77.7109375" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +480,11 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,8 +500,11 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -499,10 +518,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -516,10 +538,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -535,8 +560,11 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -551,6 +579,9 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>